<commit_message>
update notebook + notebook data
</commit_message>
<xml_diff>
--- a/examples/data/data_sectors.xlsx
+++ b/examples/data/data_sectors.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="11">
   <si>
     <t>sector</t>
   </si>
@@ -47,13 +47,25 @@
   <si>
     <t>North America</t>
   </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,7 +99,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1109,6 +1121,1254 @@
         <v>5.1262955998449423E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>3.3220564752850343</v>
+      </c>
+      <c r="D8">
+        <v>3.1503497972403762</v>
+      </c>
+      <c r="E8">
+        <v>3.0527921157410978</v>
+      </c>
+      <c r="F8">
+        <v>2.9552344342418193</v>
+      </c>
+      <c r="G8">
+        <v>2.8576767527425408</v>
+      </c>
+      <c r="H8">
+        <v>2.7601190712432624</v>
+      </c>
+      <c r="I8">
+        <v>2.6625613897439848</v>
+      </c>
+      <c r="J8">
+        <v>2.4712202694763543</v>
+      </c>
+      <c r="K8">
+        <v>2.2798791492087238</v>
+      </c>
+      <c r="L8">
+        <v>2.0885380289410933</v>
+      </c>
+      <c r="M8">
+        <v>1.897196908673463</v>
+      </c>
+      <c r="N8">
+        <v>1.7058557884058332</v>
+      </c>
+      <c r="O8">
+        <v>1.5675115369354773</v>
+      </c>
+      <c r="P8">
+        <v>1.4291672854651214</v>
+      </c>
+      <c r="Q8">
+        <v>1.2908230339947655</v>
+      </c>
+      <c r="R8">
+        <v>1.1524787825244096</v>
+      </c>
+      <c r="S8">
+        <v>1.0141345310540539</v>
+      </c>
+      <c r="T8">
+        <v>0.93135402088574104</v>
+      </c>
+      <c r="U8">
+        <v>0.84857351071742815</v>
+      </c>
+      <c r="V8">
+        <v>0.76579300054911525</v>
+      </c>
+      <c r="W8">
+        <v>0.68301249038080236</v>
+      </c>
+      <c r="X8">
+        <v>0.60023198021248958</v>
+      </c>
+      <c r="Y8">
+        <v>0.54764381180586075</v>
+      </c>
+      <c r="Z8">
+        <v>0.49505564339923191</v>
+      </c>
+      <c r="AA8">
+        <v>0.44246747499260308</v>
+      </c>
+      <c r="AB8">
+        <v>0.38987930658597425</v>
+      </c>
+      <c r="AC8">
+        <v>0.33729113817934536</v>
+      </c>
+      <c r="AD8">
+        <v>0.30183295169109542</v>
+      </c>
+      <c r="AE8">
+        <v>0.26637476520284548</v>
+      </c>
+      <c r="AF8">
+        <v>0.23091657871459553</v>
+      </c>
+      <c r="AG8">
+        <v>0.19545839222634559</v>
+      </c>
+      <c r="AH8">
+        <v>0.16000020573809565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3.1312119625647341</v>
+      </c>
+      <c r="D9">
+        <v>2.9869966982706138</v>
+      </c>
+      <c r="E9">
+        <v>2.8847804173877667</v>
+      </c>
+      <c r="F9">
+        <v>2.7825641365049196</v>
+      </c>
+      <c r="G9">
+        <v>2.6803478556220726</v>
+      </c>
+      <c r="H9">
+        <v>2.5781315747392255</v>
+      </c>
+      <c r="I9">
+        <v>2.4759152938563789</v>
+      </c>
+      <c r="J9">
+        <v>2.2910527372934544</v>
+      </c>
+      <c r="K9">
+        <v>2.1061901807305299</v>
+      </c>
+      <c r="L9">
+        <v>1.9213276241676056</v>
+      </c>
+      <c r="M9">
+        <v>1.7364650676046813</v>
+      </c>
+      <c r="N9">
+        <v>1.5516025110417573</v>
+      </c>
+      <c r="O9">
+        <v>1.432600820509025</v>
+      </c>
+      <c r="P9">
+        <v>1.3135991299762928</v>
+      </c>
+      <c r="Q9">
+        <v>1.1945974394435606</v>
+      </c>
+      <c r="R9">
+        <v>1.0755957489108283</v>
+      </c>
+      <c r="S9">
+        <v>0.95659405837809663</v>
+      </c>
+      <c r="T9">
+        <v>0.87733272301640342</v>
+      </c>
+      <c r="U9">
+        <v>0.7980713876547102</v>
+      </c>
+      <c r="V9">
+        <v>0.71881005229301698</v>
+      </c>
+      <c r="W9">
+        <v>0.63954871693132376</v>
+      </c>
+      <c r="X9">
+        <v>0.56028738156963076</v>
+      </c>
+      <c r="Y9">
+        <v>0.51636746197127092</v>
+      </c>
+      <c r="Z9">
+        <v>0.47244754237291103</v>
+      </c>
+      <c r="AA9">
+        <v>0.42852762277455114</v>
+      </c>
+      <c r="AB9">
+        <v>0.38460770317619125</v>
+      </c>
+      <c r="AC9">
+        <v>0.34068778357783136</v>
+      </c>
+      <c r="AD9">
+        <v>0.30455031546034383</v>
+      </c>
+      <c r="AE9">
+        <v>0.26841284734285631</v>
+      </c>
+      <c r="AF9">
+        <v>0.23227537922536876</v>
+      </c>
+      <c r="AG9">
+        <v>0.1961379111078812</v>
+      </c>
+      <c r="AH9">
+        <v>0.16000044299039362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2.9870685915231707</v>
+      </c>
+      <c r="D10">
+        <v>2.9486311713663316</v>
+      </c>
+      <c r="E10">
+        <v>2.9113425981015508</v>
+      </c>
+      <c r="F10">
+        <v>2.8740540248367701</v>
+      </c>
+      <c r="G10">
+        <v>2.8367654515719893</v>
+      </c>
+      <c r="H10">
+        <v>2.7994768783072086</v>
+      </c>
+      <c r="I10">
+        <v>2.9727829014739982</v>
+      </c>
+      <c r="J10">
+        <v>2.8314755601186952</v>
+      </c>
+      <c r="K10">
+        <v>2.6901682187633922</v>
+      </c>
+      <c r="L10">
+        <v>2.5488608774080892</v>
+      </c>
+      <c r="M10">
+        <v>2.4075535360527862</v>
+      </c>
+      <c r="N10">
+        <v>2.2662461946974841</v>
+      </c>
+      <c r="O10">
+        <v>2.1619493306345343</v>
+      </c>
+      <c r="P10">
+        <v>2.0576524665715845</v>
+      </c>
+      <c r="Q10">
+        <v>1.9533556025086347</v>
+      </c>
+      <c r="R10">
+        <v>1.8490587384456849</v>
+      </c>
+      <c r="S10">
+        <v>1.7447618743827347</v>
+      </c>
+      <c r="T10">
+        <v>1.6053321610476659</v>
+      </c>
+      <c r="U10">
+        <v>1.465902447712597</v>
+      </c>
+      <c r="V10">
+        <v>1.3264727343775282</v>
+      </c>
+      <c r="W10">
+        <v>1.1870430210424594</v>
+      </c>
+      <c r="X10">
+        <v>1.0476133077073908</v>
+      </c>
+      <c r="Y10">
+        <v>0.95512048921799952</v>
+      </c>
+      <c r="Z10">
+        <v>0.86262767072860824</v>
+      </c>
+      <c r="AA10">
+        <v>0.77013485223921696</v>
+      </c>
+      <c r="AB10">
+        <v>0.67764203374982568</v>
+      </c>
+      <c r="AC10">
+        <v>0.58514921526043429</v>
+      </c>
+      <c r="AD10">
+        <v>0.50012180186755084</v>
+      </c>
+      <c r="AE10">
+        <v>0.41509438847466734</v>
+      </c>
+      <c r="AF10">
+        <v>0.33006697508178384</v>
+      </c>
+      <c r="AG10">
+        <v>0.24503956168890034</v>
+      </c>
+      <c r="AH10">
+        <v>0.16001214829601679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0.60756037313049427</v>
+      </c>
+      <c r="D11">
+        <v>0.45274433529466107</v>
+      </c>
+      <c r="E11">
+        <v>0.41508425410495076</v>
+      </c>
+      <c r="F11">
+        <v>0.37742417291524044</v>
+      </c>
+      <c r="G11">
+        <v>0.33976409172553013</v>
+      </c>
+      <c r="H11">
+        <v>0.30210401053581981</v>
+      </c>
+      <c r="I11">
+        <v>0.26444392934610944</v>
+      </c>
+      <c r="J11">
+        <v>0.23622922761637988</v>
+      </c>
+      <c r="K11">
+        <v>0.20801452588665031</v>
+      </c>
+      <c r="L11">
+        <v>0.17979982415692075</v>
+      </c>
+      <c r="M11">
+        <v>0.15158512242719119</v>
+      </c>
+      <c r="N11">
+        <v>0.12337042069746158</v>
+      </c>
+      <c r="O11">
+        <v>0.10876688805755423</v>
+      </c>
+      <c r="P11">
+        <v>9.416335541764688E-2</v>
+      </c>
+      <c r="Q11">
+        <v>7.9559822777739528E-2</v>
+      </c>
+      <c r="R11">
+        <v>6.4956290137832176E-2</v>
+      </c>
+      <c r="S11">
+        <v>5.035275749792479E-2</v>
+      </c>
+      <c r="T11">
+        <v>4.4370914073610171E-2</v>
+      </c>
+      <c r="U11">
+        <v>3.8389070649295559E-2</v>
+      </c>
+      <c r="V11">
+        <v>3.2407227224980947E-2</v>
+      </c>
+      <c r="W11">
+        <v>2.6425383800666332E-2</v>
+      </c>
+      <c r="X11">
+        <v>2.0443540376351713E-2</v>
+      </c>
+      <c r="Y11">
+        <v>1.8318493555452481E-2</v>
+      </c>
+      <c r="Z11">
+        <v>1.6193446734553248E-2</v>
+      </c>
+      <c r="AA11">
+        <v>1.4068399913654016E-2</v>
+      </c>
+      <c r="AB11">
+        <v>1.1943353092754783E-2</v>
+      </c>
+      <c r="AC11">
+        <v>9.818306271855556E-3</v>
+      </c>
+      <c r="AD11">
+        <v>8.6526746345105456E-3</v>
+      </c>
+      <c r="AE11">
+        <v>7.4870429971655361E-3</v>
+      </c>
+      <c r="AF11">
+        <v>6.3214113598205265E-3</v>
+      </c>
+      <c r="AG11">
+        <v>5.155779722475517E-3</v>
+      </c>
+      <c r="AH11">
+        <v>3.9901480851305075E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0.35881498057849487</v>
+      </c>
+      <c r="D12">
+        <v>0.28654682330797321</v>
+      </c>
+      <c r="E12">
+        <v>0.26075570258778741</v>
+      </c>
+      <c r="F12">
+        <v>0.23496458186760161</v>
+      </c>
+      <c r="G12">
+        <v>0.20917346114741581</v>
+      </c>
+      <c r="H12">
+        <v>0.18338234042723001</v>
+      </c>
+      <c r="I12">
+        <v>0.15759121970704418</v>
+      </c>
+      <c r="J12">
+        <v>0.14282943407381637</v>
+      </c>
+      <c r="K12">
+        <v>0.12806764844058857</v>
+      </c>
+      <c r="L12">
+        <v>0.11330586280736078</v>
+      </c>
+      <c r="M12">
+        <v>9.8544077174132994E-2</v>
+      </c>
+      <c r="N12">
+        <v>8.3782291540905204E-2</v>
+      </c>
+      <c r="O12">
+        <v>7.7461601465999855E-2</v>
+      </c>
+      <c r="P12">
+        <v>7.1140911391094505E-2</v>
+      </c>
+      <c r="Q12">
+        <v>6.4820221316189156E-2</v>
+      </c>
+      <c r="R12">
+        <v>5.8499531241283813E-2</v>
+      </c>
+      <c r="S12">
+        <v>5.2178841166378484E-2</v>
+      </c>
+      <c r="T12">
+        <v>4.6847554066451039E-2</v>
+      </c>
+      <c r="U12">
+        <v>4.1516266966523593E-2</v>
+      </c>
+      <c r="V12">
+        <v>3.6184979866596148E-2</v>
+      </c>
+      <c r="W12">
+        <v>3.0853692766668699E-2</v>
+      </c>
+      <c r="X12">
+        <v>2.552240566674124E-2</v>
+      </c>
+      <c r="Y12">
+        <v>2.2743070565822931E-2</v>
+      </c>
+      <c r="Z12">
+        <v>1.9963735464904622E-2</v>
+      </c>
+      <c r="AA12">
+        <v>1.7184400363986312E-2</v>
+      </c>
+      <c r="AB12">
+        <v>1.4405065263068003E-2</v>
+      </c>
+      <c r="AC12">
+        <v>1.1625730162149695E-2</v>
+      </c>
+      <c r="AD12">
+        <v>1.0380657217094009E-2</v>
+      </c>
+      <c r="AE12">
+        <v>9.1355842720383228E-3</v>
+      </c>
+      <c r="AF12">
+        <v>7.8905113269826365E-3</v>
+      </c>
+      <c r="AG12">
+        <v>6.6454383819269502E-3</v>
+      </c>
+      <c r="AH12">
+        <v>5.4003654368712638E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0.41259349875015872</v>
+      </c>
+      <c r="D13">
+        <v>0.38454300118653756</v>
+      </c>
+      <c r="E13">
+        <v>0.33745768973131279</v>
+      </c>
+      <c r="F13">
+        <v>0.29037237827608803</v>
+      </c>
+      <c r="G13">
+        <v>0.24328706682086326</v>
+      </c>
+      <c r="H13">
+        <v>0.1962017553656385</v>
+      </c>
+      <c r="I13">
+        <v>0.19231409082406881</v>
+      </c>
+      <c r="J13">
+        <v>0.16704492796205822</v>
+      </c>
+      <c r="K13">
+        <v>0.14177576510004763</v>
+      </c>
+      <c r="L13">
+        <v>0.11650660223803705</v>
+      </c>
+      <c r="M13">
+        <v>9.1237439376026463E-2</v>
+      </c>
+      <c r="N13">
+        <v>6.596827651401585E-2</v>
+      </c>
+      <c r="O13">
+        <v>6.0146071842620982E-2</v>
+      </c>
+      <c r="P13">
+        <v>5.4323867171226115E-2</v>
+      </c>
+      <c r="Q13">
+        <v>4.8501662499831247E-2</v>
+      </c>
+      <c r="R13">
+        <v>4.2679457828436379E-2</v>
+      </c>
+      <c r="S13">
+        <v>3.6857253157041525E-2</v>
+      </c>
+      <c r="T13">
+        <v>3.39296363678427E-2</v>
+      </c>
+      <c r="U13">
+        <v>3.1002019578643875E-2</v>
+      </c>
+      <c r="V13">
+        <v>2.8074402789445049E-2</v>
+      </c>
+      <c r="W13">
+        <v>2.5146786000246224E-2</v>
+      </c>
+      <c r="X13">
+        <v>2.2219169211047399E-2</v>
+      </c>
+      <c r="Y13">
+        <v>1.8843767894743155E-2</v>
+      </c>
+      <c r="Z13">
+        <v>1.5468366578438914E-2</v>
+      </c>
+      <c r="AA13">
+        <v>1.2092965262134672E-2</v>
+      </c>
+      <c r="AB13">
+        <v>8.7175639458304307E-3</v>
+      </c>
+      <c r="AC13">
+        <v>5.3421626295261882E-3</v>
+      </c>
+      <c r="AD13">
+        <v>5.2989892235899387E-3</v>
+      </c>
+      <c r="AE13">
+        <v>5.2558158176536892E-3</v>
+      </c>
+      <c r="AF13">
+        <v>5.2126424117174396E-3</v>
+      </c>
+      <c r="AG13">
+        <v>5.1694690057811901E-3</v>
+      </c>
+      <c r="AH13">
+        <v>5.1262955998449423E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>3.3220564752850343</v>
+      </c>
+      <c r="D14">
+        <v>3.1503497972403762</v>
+      </c>
+      <c r="E14">
+        <v>3.0527921157410978</v>
+      </c>
+      <c r="F14">
+        <v>2.9552344342418193</v>
+      </c>
+      <c r="G14">
+        <v>2.8576767527425408</v>
+      </c>
+      <c r="H14">
+        <v>2.7601190712432624</v>
+      </c>
+      <c r="I14">
+        <v>2.6625613897439848</v>
+      </c>
+      <c r="J14">
+        <v>2.4712202694763543</v>
+      </c>
+      <c r="K14">
+        <v>2.2798791492087238</v>
+      </c>
+      <c r="L14">
+        <v>2.0885380289410933</v>
+      </c>
+      <c r="M14">
+        <v>1.897196908673463</v>
+      </c>
+      <c r="N14">
+        <v>1.7058557884058332</v>
+      </c>
+      <c r="O14">
+        <v>1.5675115369354773</v>
+      </c>
+      <c r="P14">
+        <v>1.4291672854651214</v>
+      </c>
+      <c r="Q14">
+        <v>1.2908230339947655</v>
+      </c>
+      <c r="R14">
+        <v>1.1524787825244096</v>
+      </c>
+      <c r="S14">
+        <v>1.0141345310540539</v>
+      </c>
+      <c r="T14">
+        <v>0.93135402088574104</v>
+      </c>
+      <c r="U14">
+        <v>0.84857351071742815</v>
+      </c>
+      <c r="V14">
+        <v>0.76579300054911525</v>
+      </c>
+      <c r="W14">
+        <v>0.68301249038080236</v>
+      </c>
+      <c r="X14">
+        <v>0.60023198021248958</v>
+      </c>
+      <c r="Y14">
+        <v>0.54764381180586075</v>
+      </c>
+      <c r="Z14">
+        <v>0.49505564339923191</v>
+      </c>
+      <c r="AA14">
+        <v>0.44246747499260308</v>
+      </c>
+      <c r="AB14">
+        <v>0.38987930658597425</v>
+      </c>
+      <c r="AC14">
+        <v>0.33729113817934536</v>
+      </c>
+      <c r="AD14">
+        <v>0.30183295169109542</v>
+      </c>
+      <c r="AE14">
+        <v>0.26637476520284548</v>
+      </c>
+      <c r="AF14">
+        <v>0.23091657871459553</v>
+      </c>
+      <c r="AG14">
+        <v>0.19545839222634559</v>
+      </c>
+      <c r="AH14">
+        <v>0.16000020573809565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3.1312119625647341</v>
+      </c>
+      <c r="D15">
+        <v>2.9869966982706138</v>
+      </c>
+      <c r="E15">
+        <v>2.8847804173877667</v>
+      </c>
+      <c r="F15">
+        <v>2.7825641365049196</v>
+      </c>
+      <c r="G15">
+        <v>2.6803478556220726</v>
+      </c>
+      <c r="H15">
+        <v>2.5781315747392255</v>
+      </c>
+      <c r="I15">
+        <v>2.4759152938563789</v>
+      </c>
+      <c r="J15">
+        <v>2.2910527372934544</v>
+      </c>
+      <c r="K15">
+        <v>2.1061901807305299</v>
+      </c>
+      <c r="L15">
+        <v>1.9213276241676056</v>
+      </c>
+      <c r="M15">
+        <v>1.7364650676046813</v>
+      </c>
+      <c r="N15">
+        <v>1.5516025110417573</v>
+      </c>
+      <c r="O15">
+        <v>1.432600820509025</v>
+      </c>
+      <c r="P15">
+        <v>1.3135991299762928</v>
+      </c>
+      <c r="Q15">
+        <v>1.1945974394435606</v>
+      </c>
+      <c r="R15">
+        <v>1.0755957489108283</v>
+      </c>
+      <c r="S15">
+        <v>0.95659405837809663</v>
+      </c>
+      <c r="T15">
+        <v>0.87733272301640342</v>
+      </c>
+      <c r="U15">
+        <v>0.7980713876547102</v>
+      </c>
+      <c r="V15">
+        <v>0.71881005229301698</v>
+      </c>
+      <c r="W15">
+        <v>0.63954871693132376</v>
+      </c>
+      <c r="X15">
+        <v>0.56028738156963076</v>
+      </c>
+      <c r="Y15">
+        <v>0.51636746197127092</v>
+      </c>
+      <c r="Z15">
+        <v>0.47244754237291103</v>
+      </c>
+      <c r="AA15">
+        <v>0.42852762277455114</v>
+      </c>
+      <c r="AB15">
+        <v>0.38460770317619125</v>
+      </c>
+      <c r="AC15">
+        <v>0.34068778357783136</v>
+      </c>
+      <c r="AD15">
+        <v>0.30455031546034383</v>
+      </c>
+      <c r="AE15">
+        <v>0.26841284734285631</v>
+      </c>
+      <c r="AF15">
+        <v>0.23227537922536876</v>
+      </c>
+      <c r="AG15">
+        <v>0.1961379111078812</v>
+      </c>
+      <c r="AH15">
+        <v>0.16000044299039362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>2.9870685915231707</v>
+      </c>
+      <c r="D16">
+        <v>2.9486311713663316</v>
+      </c>
+      <c r="E16">
+        <v>2.9113425981015508</v>
+      </c>
+      <c r="F16">
+        <v>2.8740540248367701</v>
+      </c>
+      <c r="G16">
+        <v>2.8367654515719893</v>
+      </c>
+      <c r="H16">
+        <v>2.7994768783072086</v>
+      </c>
+      <c r="I16">
+        <v>2.9727829014739982</v>
+      </c>
+      <c r="J16">
+        <v>2.8314755601186952</v>
+      </c>
+      <c r="K16">
+        <v>2.6901682187633922</v>
+      </c>
+      <c r="L16">
+        <v>2.5488608774080892</v>
+      </c>
+      <c r="M16">
+        <v>2.4075535360527862</v>
+      </c>
+      <c r="N16">
+        <v>2.2662461946974841</v>
+      </c>
+      <c r="O16">
+        <v>2.1619493306345343</v>
+      </c>
+      <c r="P16">
+        <v>2.0576524665715845</v>
+      </c>
+      <c r="Q16">
+        <v>1.9533556025086347</v>
+      </c>
+      <c r="R16">
+        <v>1.8490587384456849</v>
+      </c>
+      <c r="S16">
+        <v>1.7447618743827347</v>
+      </c>
+      <c r="T16">
+        <v>1.6053321610476659</v>
+      </c>
+      <c r="U16">
+        <v>1.465902447712597</v>
+      </c>
+      <c r="V16">
+        <v>1.3264727343775282</v>
+      </c>
+      <c r="W16">
+        <v>1.1870430210424594</v>
+      </c>
+      <c r="X16">
+        <v>1.0476133077073908</v>
+      </c>
+      <c r="Y16">
+        <v>0.95512048921799952</v>
+      </c>
+      <c r="Z16">
+        <v>0.86262767072860824</v>
+      </c>
+      <c r="AA16">
+        <v>0.77013485223921696</v>
+      </c>
+      <c r="AB16">
+        <v>0.67764203374982568</v>
+      </c>
+      <c r="AC16">
+        <v>0.58514921526043429</v>
+      </c>
+      <c r="AD16">
+        <v>0.50012180186755084</v>
+      </c>
+      <c r="AE16">
+        <v>0.41509438847466734</v>
+      </c>
+      <c r="AF16">
+        <v>0.33006697508178384</v>
+      </c>
+      <c r="AG16">
+        <v>0.24503956168890034</v>
+      </c>
+      <c r="AH16">
+        <v>0.16001214829601679</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>0.60756037313049427</v>
+      </c>
+      <c r="D17">
+        <v>0.45274433529466107</v>
+      </c>
+      <c r="E17">
+        <v>0.41508425410495076</v>
+      </c>
+      <c r="F17">
+        <v>0.37742417291524044</v>
+      </c>
+      <c r="G17">
+        <v>0.33976409172553013</v>
+      </c>
+      <c r="H17">
+        <v>0.30210401053581981</v>
+      </c>
+      <c r="I17">
+        <v>0.26444392934610944</v>
+      </c>
+      <c r="J17">
+        <v>0.23622922761637988</v>
+      </c>
+      <c r="K17">
+        <v>0.20801452588665031</v>
+      </c>
+      <c r="L17">
+        <v>0.17979982415692075</v>
+      </c>
+      <c r="M17">
+        <v>0.15158512242719119</v>
+      </c>
+      <c r="N17">
+        <v>0.12337042069746158</v>
+      </c>
+      <c r="O17">
+        <v>0.10876688805755423</v>
+      </c>
+      <c r="P17">
+        <v>9.416335541764688E-2</v>
+      </c>
+      <c r="Q17">
+        <v>7.9559822777739528E-2</v>
+      </c>
+      <c r="R17">
+        <v>6.4956290137832176E-2</v>
+      </c>
+      <c r="S17">
+        <v>5.035275749792479E-2</v>
+      </c>
+      <c r="T17">
+        <v>4.4370914073610171E-2</v>
+      </c>
+      <c r="U17">
+        <v>3.8389070649295559E-2</v>
+      </c>
+      <c r="V17">
+        <v>3.2407227224980947E-2</v>
+      </c>
+      <c r="W17">
+        <v>2.6425383800666332E-2</v>
+      </c>
+      <c r="X17">
+        <v>2.0443540376351713E-2</v>
+      </c>
+      <c r="Y17">
+        <v>1.8318493555452481E-2</v>
+      </c>
+      <c r="Z17">
+        <v>1.6193446734553248E-2</v>
+      </c>
+      <c r="AA17">
+        <v>1.4068399913654016E-2</v>
+      </c>
+      <c r="AB17">
+        <v>1.1943353092754783E-2</v>
+      </c>
+      <c r="AC17">
+        <v>9.818306271855556E-3</v>
+      </c>
+      <c r="AD17">
+        <v>8.6526746345105456E-3</v>
+      </c>
+      <c r="AE17">
+        <v>7.4870429971655361E-3</v>
+      </c>
+      <c r="AF17">
+        <v>6.3214113598205265E-3</v>
+      </c>
+      <c r="AG17">
+        <v>5.155779722475517E-3</v>
+      </c>
+      <c r="AH17">
+        <v>3.9901480851305075E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>0.35881498057849487</v>
+      </c>
+      <c r="D18">
+        <v>0.28654682330797321</v>
+      </c>
+      <c r="E18">
+        <v>0.26075570258778741</v>
+      </c>
+      <c r="F18">
+        <v>0.23496458186760161</v>
+      </c>
+      <c r="G18">
+        <v>0.20917346114741581</v>
+      </c>
+      <c r="H18">
+        <v>0.18338234042723001</v>
+      </c>
+      <c r="I18">
+        <v>0.15759121970704418</v>
+      </c>
+      <c r="J18">
+        <v>0.14282943407381637</v>
+      </c>
+      <c r="K18">
+        <v>0.12806764844058857</v>
+      </c>
+      <c r="L18">
+        <v>0.11330586280736078</v>
+      </c>
+      <c r="M18">
+        <v>9.8544077174132994E-2</v>
+      </c>
+      <c r="N18">
+        <v>8.3782291540905204E-2</v>
+      </c>
+      <c r="O18">
+        <v>7.7461601465999855E-2</v>
+      </c>
+      <c r="P18">
+        <v>7.1140911391094505E-2</v>
+      </c>
+      <c r="Q18">
+        <v>6.4820221316189156E-2</v>
+      </c>
+      <c r="R18">
+        <v>5.8499531241283813E-2</v>
+      </c>
+      <c r="S18">
+        <v>5.2178841166378484E-2</v>
+      </c>
+      <c r="T18">
+        <v>4.6847554066451039E-2</v>
+      </c>
+      <c r="U18">
+        <v>4.1516266966523593E-2</v>
+      </c>
+      <c r="V18">
+        <v>3.6184979866596148E-2</v>
+      </c>
+      <c r="W18">
+        <v>3.0853692766668699E-2</v>
+      </c>
+      <c r="X18">
+        <v>2.552240566674124E-2</v>
+      </c>
+      <c r="Y18">
+        <v>2.2743070565822931E-2</v>
+      </c>
+      <c r="Z18">
+        <v>1.9963735464904622E-2</v>
+      </c>
+      <c r="AA18">
+        <v>1.7184400363986312E-2</v>
+      </c>
+      <c r="AB18">
+        <v>1.4405065263068003E-2</v>
+      </c>
+      <c r="AC18">
+        <v>1.1625730162149695E-2</v>
+      </c>
+      <c r="AD18">
+        <v>1.0380657217094009E-2</v>
+      </c>
+      <c r="AE18">
+        <v>9.1355842720383228E-3</v>
+      </c>
+      <c r="AF18">
+        <v>7.8905113269826365E-3</v>
+      </c>
+      <c r="AG18">
+        <v>6.6454383819269502E-3</v>
+      </c>
+      <c r="AH18">
+        <v>5.4003654368712638E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>0.41259349875015872</v>
+      </c>
+      <c r="D19">
+        <v>0.38454300118653756</v>
+      </c>
+      <c r="E19">
+        <v>0.33745768973131279</v>
+      </c>
+      <c r="F19">
+        <v>0.29037237827608803</v>
+      </c>
+      <c r="G19">
+        <v>0.24328706682086326</v>
+      </c>
+      <c r="H19">
+        <v>0.1962017553656385</v>
+      </c>
+      <c r="I19">
+        <v>0.19231409082406881</v>
+      </c>
+      <c r="J19">
+        <v>0.16704492796205822</v>
+      </c>
+      <c r="K19">
+        <v>0.14177576510004763</v>
+      </c>
+      <c r="L19">
+        <v>0.11650660223803705</v>
+      </c>
+      <c r="M19">
+        <v>9.1237439376026463E-2</v>
+      </c>
+      <c r="N19">
+        <v>6.596827651401585E-2</v>
+      </c>
+      <c r="O19">
+        <v>6.0146071842620982E-2</v>
+      </c>
+      <c r="P19">
+        <v>5.4323867171226115E-2</v>
+      </c>
+      <c r="Q19">
+        <v>4.8501662499831247E-2</v>
+      </c>
+      <c r="R19">
+        <v>4.2679457828436379E-2</v>
+      </c>
+      <c r="S19">
+        <v>3.6857253157041525E-2</v>
+      </c>
+      <c r="T19">
+        <v>3.39296363678427E-2</v>
+      </c>
+      <c r="U19">
+        <v>3.1002019578643875E-2</v>
+      </c>
+      <c r="V19">
+        <v>2.8074402789445049E-2</v>
+      </c>
+      <c r="W19">
+        <v>2.5146786000246224E-2</v>
+      </c>
+      <c r="X19">
+        <v>2.2219169211047399E-2</v>
+      </c>
+      <c r="Y19">
+        <v>1.8843767894743155E-2</v>
+      </c>
+      <c r="Z19">
+        <v>1.5468366578438914E-2</v>
+      </c>
+      <c r="AA19">
+        <v>1.2092965262134672E-2</v>
+      </c>
+      <c r="AB19">
+        <v>8.7175639458304307E-3</v>
+      </c>
+      <c r="AC19">
+        <v>5.3421626295261882E-3</v>
+      </c>
+      <c r="AD19">
+        <v>5.2989892235899387E-3</v>
+      </c>
+      <c r="AE19">
+        <v>5.2558158176536892E-3</v>
+      </c>
+      <c r="AF19">
+        <v>5.2126424117174396E-3</v>
+      </c>
+      <c r="AG19">
+        <v>5.1694690057811901E-3</v>
+      </c>
+      <c r="AH19">
+        <v>5.1262955998449423E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1116,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C7" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1859,6 +3119,1254 @@
         <v>3.2269880188280364E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.4000130214877569E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-7.6398544753241149E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="R11" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="S11" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="T11" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="U11" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="V11" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="W11" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="X11" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.5000548791797463E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-7.6445097814137997E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="R12" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="S12" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="W12" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="X12" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AH12" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.0000446929317572E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-7.581010331041782E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="R13" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="S13" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="T13" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="U13" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="V13" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="W13" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="W16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="X16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.4000130214877569E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-7.6398544753241149E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5.9958359610187584E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="M17" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>4.8590152054553304E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="R17" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="S17" s="2">
+        <v>4.6143303388171741E-2</v>
+      </c>
+      <c r="T17" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="U17" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="V17" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="W17" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="X17" s="2">
+        <v>4.0092355172694383E-2</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>2.5847885659444403E-2</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>1.1912758443362925E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.5000548791797463E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-7.6445097814137997E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2.5801327618059089E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="M18" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>4.0021273806288837E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="P18" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="S18" s="2">
+        <v>3.6938283793271909E-2</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="X18" s="2">
+        <v>1.8701956793973018E-2</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>1.2045554009002979E-2</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>6.3601028128394965E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.0000446929317572E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-7.581010331041782E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.9813190643994671E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <v>3.1877741268007798E-2</v>
+      </c>
+      <c r="O19" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="P19" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="R19" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="S19" s="2">
+        <v>2.1494276219452768E-2</v>
+      </c>
+      <c r="T19" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="U19" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="V19" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="W19" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="X19" s="2">
+        <v>3.420717440226384E-2</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>1.4292979405873707E-2</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AG19" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>3.2269880188280364E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>